<commit_message>
Fix rental data import logic and update Excel file
- Corrected import service to properly map proprietors by name instead of ID order
- Fixed header parsing to extract column names from the correct Excel structure
- Updated dashboard calculations to use unique property values (avoiding duplicates)
- Removed duplicate Excel file and updated main rental data file
- Successfully imported 1710 rental records from Jan-Sep 2025
</commit_message>
<xml_diff>
--- a/Alugueis.xlsx
+++ b/Alugueis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcozz\Desktop\Proyecto Alquiler\Proyecto V2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcozz\Desktop\Proyecto Alquiler\Proyecto V4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96522CE0-374B-43FC-B2D5-8A57A3A532D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02083F2-3D44-4676-8E36-A2028D804743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="1" activeTab="8" xr2:uid="{B6C19694-A322-4A67-A72C-FBDA8501CAA3}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="2" activeTab="9" xr2:uid="{B6C19694-A322-4A67-A72C-FBDA8501CAA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Jan2025" sheetId="8" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="Jul2025" sheetId="3" r:id="rId7"/>
     <sheet name="Ago2025" sheetId="10" r:id="rId8"/>
     <sheet name="Set2025" sheetId="11" r:id="rId9"/>
+    <sheet name="Out25" sheetId="12" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="31">
   <si>
     <t>Dep. Lacerda</t>
   </si>
@@ -1403,6 +1404,850 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCB330C3-BDFF-4A88-8B6B-49AF57B5A231}">
+  <dimension ref="A1:M20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="11" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A1" s="5">
+        <v>45931</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="4">
+        <v>14713.62</v>
+      </c>
+      <c r="C2" s="4">
+        <v>3597.2474999999999</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1235.1524999999999</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1235.1524999999999</v>
+      </c>
+      <c r="F2" s="4">
+        <v>1235.1524999999999</v>
+      </c>
+      <c r="G2" s="4">
+        <v>1852.72875</v>
+      </c>
+      <c r="H2" s="4">
+        <v>1852.72875</v>
+      </c>
+      <c r="I2" s="4">
+        <v>617.57624999999973</v>
+      </c>
+      <c r="J2" s="4">
+        <v>617.57624999999973</v>
+      </c>
+      <c r="K2" s="4">
+        <v>1235.1524999999995</v>
+      </c>
+      <c r="L2" s="4">
+        <v>1235.1524999999995</v>
+      </c>
+      <c r="M2" s="4">
+        <v>1003.59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="4">
+        <v>53765.829999999994</v>
+      </c>
+      <c r="C3" s="4">
+        <v>6458.2937499999998</v>
+      </c>
+      <c r="D3" s="4">
+        <v>4208.6076388888887</v>
+      </c>
+      <c r="E3" s="4">
+        <v>4023.9476388888888</v>
+      </c>
+      <c r="F3" s="4">
+        <v>4208.6076388888887</v>
+      </c>
+      <c r="G3" s="4">
+        <v>8252.2983333333323</v>
+      </c>
+      <c r="H3" s="4">
+        <v>8252.4383333333335</v>
+      </c>
+      <c r="I3" s="4">
+        <v>3320.5661111111076</v>
+      </c>
+      <c r="J3" s="4">
+        <v>3320.5661111111076</v>
+      </c>
+      <c r="K3" s="4">
+        <v>5860.2522222222151</v>
+      </c>
+      <c r="L3" s="4">
+        <v>5860.2522222222151</v>
+      </c>
+      <c r="M3" s="4">
+        <v>3189.68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4">
+        <v>5933.32</v>
+      </c>
+      <c r="C4" s="4">
+        <v>741.66499999999996</v>
+      </c>
+      <c r="D4" s="4">
+        <v>412.0361111111111</v>
+      </c>
+      <c r="E4" s="4">
+        <v>412.0361111111111</v>
+      </c>
+      <c r="F4" s="4">
+        <v>412.0361111111111</v>
+      </c>
+      <c r="G4" s="4">
+        <v>988.88666666666654</v>
+      </c>
+      <c r="H4" s="4">
+        <v>988.88666666666654</v>
+      </c>
+      <c r="I4" s="4">
+        <v>329.62888888888847</v>
+      </c>
+      <c r="J4" s="4">
+        <v>329.62888888888847</v>
+      </c>
+      <c r="K4" s="4">
+        <v>659.25777777777694</v>
+      </c>
+      <c r="L4" s="4">
+        <v>659.25777777777694</v>
+      </c>
+      <c r="M4" s="4">
+        <v>488.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4">
+        <v>2748.8500000000004</v>
+      </c>
+      <c r="C5" s="4">
+        <v>343.60625000000005</v>
+      </c>
+      <c r="D5" s="4">
+        <v>190.89236111111111</v>
+      </c>
+      <c r="E5" s="4">
+        <v>190.89236111111111</v>
+      </c>
+      <c r="F5" s="4">
+        <v>190.89236111111111</v>
+      </c>
+      <c r="G5" s="4">
+        <v>458.14166666666665</v>
+      </c>
+      <c r="H5" s="4">
+        <v>458.14166666666665</v>
+      </c>
+      <c r="I5" s="4">
+        <v>152.71388888888873</v>
+      </c>
+      <c r="J5" s="4">
+        <v>152.71388888888873</v>
+      </c>
+      <c r="K5" s="4">
+        <v>305.42777777777746</v>
+      </c>
+      <c r="L5" s="4">
+        <v>305.42777777777746</v>
+      </c>
+      <c r="M5" s="4">
+        <v>177.68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="4">
+        <v>2627.5</v>
+      </c>
+      <c r="C6" s="4">
+        <v>328.4375</v>
+      </c>
+      <c r="D6" s="4">
+        <v>182.46527777777777</v>
+      </c>
+      <c r="E6" s="4">
+        <v>182.46527777777777</v>
+      </c>
+      <c r="F6" s="4">
+        <v>182.46527777777777</v>
+      </c>
+      <c r="G6" s="4">
+        <v>437.91666666666663</v>
+      </c>
+      <c r="H6" s="4">
+        <v>437.91666666666663</v>
+      </c>
+      <c r="I6" s="4">
+        <v>145.97222222222206</v>
+      </c>
+      <c r="J6" s="4">
+        <v>145.97222222222206</v>
+      </c>
+      <c r="K6" s="4">
+        <v>291.94444444444412</v>
+      </c>
+      <c r="L6" s="4">
+        <v>291.94444444444412</v>
+      </c>
+      <c r="M6" s="4">
+        <v>175.99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="4">
+        <v>2542.96</v>
+      </c>
+      <c r="C7" s="4">
+        <v>317.87</v>
+      </c>
+      <c r="D7" s="4">
+        <v>176.59444444444443</v>
+      </c>
+      <c r="E7" s="4">
+        <v>176.59444444444443</v>
+      </c>
+      <c r="F7" s="4">
+        <v>176.59444444444443</v>
+      </c>
+      <c r="G7" s="4">
+        <v>423.82666666666665</v>
+      </c>
+      <c r="H7" s="4">
+        <v>423.82666666666665</v>
+      </c>
+      <c r="I7" s="4">
+        <v>141.2755555555554</v>
+      </c>
+      <c r="J7" s="4">
+        <v>141.2755555555554</v>
+      </c>
+      <c r="K7" s="4">
+        <v>282.5511111111108</v>
+      </c>
+      <c r="L7" s="4">
+        <v>282.5511111111108</v>
+      </c>
+      <c r="M7" s="4">
+        <v>157.18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="4">
+        <v>2043.06</v>
+      </c>
+      <c r="C8" s="4">
+        <v>255.38249999999999</v>
+      </c>
+      <c r="D8" s="4">
+        <v>141.87916666666666</v>
+      </c>
+      <c r="E8" s="4">
+        <v>141.87916666666666</v>
+      </c>
+      <c r="F8" s="4">
+        <v>141.87916666666666</v>
+      </c>
+      <c r="G8" s="4">
+        <v>340.51</v>
+      </c>
+      <c r="H8" s="4">
+        <v>340.51</v>
+      </c>
+      <c r="I8" s="4">
+        <v>113.50333333333322</v>
+      </c>
+      <c r="J8" s="4">
+        <v>113.50333333333322</v>
+      </c>
+      <c r="K8" s="4">
+        <v>227.00666666666643</v>
+      </c>
+      <c r="L8" s="4">
+        <v>227.00666666666643</v>
+      </c>
+      <c r="M8" s="4">
+        <v>125.71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="4">
+        <v>2035.44</v>
+      </c>
+      <c r="C9" s="4">
+        <v>254.43</v>
+      </c>
+      <c r="D9" s="4">
+        <v>141.35</v>
+      </c>
+      <c r="E9" s="4">
+        <v>141.35</v>
+      </c>
+      <c r="F9" s="4">
+        <v>141.35</v>
+      </c>
+      <c r="G9" s="4">
+        <v>339.23999999999995</v>
+      </c>
+      <c r="H9" s="4">
+        <v>339.23999999999995</v>
+      </c>
+      <c r="I9" s="4">
+        <v>113.07999999999988</v>
+      </c>
+      <c r="J9" s="4">
+        <v>113.07999999999988</v>
+      </c>
+      <c r="K9" s="4">
+        <v>226.15999999999977</v>
+      </c>
+      <c r="L9" s="4">
+        <v>226.15999999999977</v>
+      </c>
+      <c r="M9" s="4">
+        <v>133.33000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="4">
+        <v>2858.98</v>
+      </c>
+      <c r="C10" s="4">
+        <v>357.3725</v>
+      </c>
+      <c r="D10" s="4">
+        <v>198.54027777777782</v>
+      </c>
+      <c r="E10" s="4">
+        <v>198.54027777777782</v>
+      </c>
+      <c r="F10" s="4">
+        <v>198.54027777777782</v>
+      </c>
+      <c r="G10" s="4">
+        <v>476.49666666666661</v>
+      </c>
+      <c r="H10" s="4">
+        <v>476.49666666666661</v>
+      </c>
+      <c r="I10" s="4">
+        <v>158.83222222222207</v>
+      </c>
+      <c r="J10" s="4">
+        <v>158.83222222222207</v>
+      </c>
+      <c r="K10" s="4">
+        <v>317.66444444444414</v>
+      </c>
+      <c r="L10" s="4">
+        <v>317.66444444444414</v>
+      </c>
+      <c r="M10" s="4">
+        <v>253.78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="4">
+        <v>-1863.76</v>
+      </c>
+      <c r="C11" s="4">
+        <v>-232.97</v>
+      </c>
+      <c r="D11" s="4">
+        <v>-129.42777777777778</v>
+      </c>
+      <c r="E11" s="4">
+        <v>-129.42777777777778</v>
+      </c>
+      <c r="F11" s="4">
+        <v>-129.42777777777778</v>
+      </c>
+      <c r="G11" s="4">
+        <v>-310.62666666666667</v>
+      </c>
+      <c r="H11" s="4">
+        <v>-310.62666666666667</v>
+      </c>
+      <c r="I11" s="4">
+        <v>-103.54222222222211</v>
+      </c>
+      <c r="J11" s="4">
+        <v>-103.54222222222211</v>
+      </c>
+      <c r="K11" s="4">
+        <v>-207.08444444444422</v>
+      </c>
+      <c r="L11" s="4">
+        <v>-207.08444444444422</v>
+      </c>
+      <c r="M11" s="4">
+        <v>88.75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0</v>
+      </c>
+      <c r="G12" s="4">
+        <v>0</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0</v>
+      </c>
+      <c r="I12" s="4">
+        <v>0</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0</v>
+      </c>
+      <c r="K12" s="4">
+        <v>0</v>
+      </c>
+      <c r="L12" s="4">
+        <v>0</v>
+      </c>
+      <c r="M12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="4">
+        <v>-524.93000000000006</v>
+      </c>
+      <c r="C13" s="4">
+        <v>-65.616250000000008</v>
+      </c>
+      <c r="D13" s="4">
+        <v>-36.453472222222224</v>
+      </c>
+      <c r="E13" s="4">
+        <v>-36.453472222222224</v>
+      </c>
+      <c r="F13" s="4">
+        <v>-36.453472222222224</v>
+      </c>
+      <c r="G13" s="4">
+        <v>-87.48833333333333</v>
+      </c>
+      <c r="H13" s="4">
+        <v>-87.48833333333333</v>
+      </c>
+      <c r="I13" s="4">
+        <v>-29.162777777777748</v>
+      </c>
+      <c r="J13" s="4">
+        <v>-29.162777777777748</v>
+      </c>
+      <c r="K13" s="4">
+        <v>-58.325555555555496</v>
+      </c>
+      <c r="L13" s="4">
+        <v>-58.325555555555496</v>
+      </c>
+      <c r="M13" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="4">
+        <v>-527.49</v>
+      </c>
+      <c r="C14" s="4">
+        <v>-65.936250000000001</v>
+      </c>
+      <c r="D14" s="4">
+        <v>-36.631250000000001</v>
+      </c>
+      <c r="E14" s="4">
+        <v>-36.631250000000001</v>
+      </c>
+      <c r="F14" s="4">
+        <v>-36.631250000000001</v>
+      </c>
+      <c r="G14" s="4">
+        <v>-87.914999999999992</v>
+      </c>
+      <c r="H14" s="4">
+        <v>-87.914999999999992</v>
+      </c>
+      <c r="I14" s="4">
+        <v>-29.304999999999968</v>
+      </c>
+      <c r="J14" s="4">
+        <v>-29.304999999999968</v>
+      </c>
+      <c r="K14" s="4">
+        <v>-58.609999999999935</v>
+      </c>
+      <c r="L14" s="4">
+        <v>-58.609999999999935</v>
+      </c>
+      <c r="M14" s="4">
+        <v>25.15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="4">
+        <v>-2450.4199999999996</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0</v>
+      </c>
+      <c r="D15" s="4">
+        <v>-272.26888888888857</v>
+      </c>
+      <c r="E15" s="4">
+        <v>-272.26888888888857</v>
+      </c>
+      <c r="F15" s="4">
+        <v>-272.26888888888857</v>
+      </c>
+      <c r="G15" s="4">
+        <v>-408.4033333333341</v>
+      </c>
+      <c r="H15" s="4">
+        <v>-408.4033333333341</v>
+      </c>
+      <c r="I15" s="4">
+        <v>-136.13444444444428</v>
+      </c>
+      <c r="J15" s="4">
+        <v>-136.13444444444428</v>
+      </c>
+      <c r="K15" s="4">
+        <v>-272.26888888888857</v>
+      </c>
+      <c r="L15" s="4">
+        <v>-272.26888888888857</v>
+      </c>
+      <c r="M15" s="4">
+        <v>116.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="4">
+        <v>1147.3899999999981</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0</v>
+      </c>
+      <c r="D16" s="4">
+        <v>127.48777777777744</v>
+      </c>
+      <c r="E16" s="4">
+        <v>127.48777777777744</v>
+      </c>
+      <c r="F16" s="4">
+        <v>127.48777777777744</v>
+      </c>
+      <c r="G16" s="4">
+        <v>191.23166666666683</v>
+      </c>
+      <c r="H16" s="4">
+        <v>191.23166666666683</v>
+      </c>
+      <c r="I16" s="4">
+        <v>63.743888888888719</v>
+      </c>
+      <c r="J16" s="4">
+        <v>63.743888888888719</v>
+      </c>
+      <c r="K16" s="4">
+        <v>127.48777777777744</v>
+      </c>
+      <c r="L16" s="4">
+        <v>127.48777777777744</v>
+      </c>
+      <c r="M16" s="4">
+        <v>942.69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="4">
+        <v>15019.99</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0</v>
+      </c>
+      <c r="D17" s="4">
+        <v>10013.326666666655</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0</v>
+      </c>
+      <c r="G17" s="4">
+        <v>2503.3316666666715</v>
+      </c>
+      <c r="H17" s="4">
+        <v>2503.3316666666715</v>
+      </c>
+      <c r="I17" s="4">
+        <v>0</v>
+      </c>
+      <c r="J17" s="4">
+        <v>0</v>
+      </c>
+      <c r="K17" s="4">
+        <v>0</v>
+      </c>
+      <c r="L17" s="4">
+        <v>0</v>
+      </c>
+      <c r="M17" s="4">
+        <v>928.77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A18" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="4">
+        <v>-2669.37</v>
+      </c>
+      <c r="C18" s="4">
+        <v>-1334.6849999999999</v>
+      </c>
+      <c r="D18" s="4">
+        <v>-444.89499999999992</v>
+      </c>
+      <c r="E18" s="4">
+        <v>-444.89499999999992</v>
+      </c>
+      <c r="F18" s="4">
+        <v>-444.89499999999992</v>
+      </c>
+      <c r="G18" s="4">
+        <v>0</v>
+      </c>
+      <c r="H18" s="4">
+        <v>0</v>
+      </c>
+      <c r="I18" s="4">
+        <v>0</v>
+      </c>
+      <c r="J18" s="4">
+        <v>0</v>
+      </c>
+      <c r="K18" s="4">
+        <v>0</v>
+      </c>
+      <c r="L18" s="4">
+        <v>0</v>
+      </c>
+      <c r="M18" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="4">
+        <v>10504.48</v>
+      </c>
+      <c r="C19" s="4">
+        <v>4980.8450000000003</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1841.211666666667</v>
+      </c>
+      <c r="E19" s="4">
+        <v>1841.211666666667</v>
+      </c>
+      <c r="F19" s="4">
+        <v>1841.211666666667</v>
+      </c>
+      <c r="G19" s="4">
+        <v>0</v>
+      </c>
+      <c r="H19" s="4">
+        <v>0</v>
+      </c>
+      <c r="I19" s="4">
+        <v>0</v>
+      </c>
+      <c r="J19" s="4">
+        <v>0</v>
+      </c>
+      <c r="K19" s="4">
+        <v>0</v>
+      </c>
+      <c r="L19" s="4">
+        <v>0</v>
+      </c>
+      <c r="M19" s="4">
+        <v>723.64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="4">
+        <v>4584.54</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0</v>
+      </c>
+      <c r="D20" s="4">
+        <v>2292.27</v>
+      </c>
+      <c r="E20" s="4">
+        <v>2292.27</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0</v>
+      </c>
+      <c r="G20" s="4">
+        <v>0</v>
+      </c>
+      <c r="H20" s="4">
+        <v>0</v>
+      </c>
+      <c r="I20" s="4">
+        <v>0</v>
+      </c>
+      <c r="J20" s="4">
+        <v>0</v>
+      </c>
+      <c r="K20" s="4">
+        <v>0</v>
+      </c>
+      <c r="L20" s="4">
+        <v>0</v>
+      </c>
+      <c r="M20" s="4">
+        <v>295.45999999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64ADDF48-3620-417A-B515-1893152E6802}">
   <dimension ref="A1:M20"/>
@@ -7320,7 +8165,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06B75B0A-505B-4FDF-A7BB-2995889744D2}">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>

</xml_diff>